<commit_message>
feat: Correção de uso do ID e Implementação dos dados na Tabela
</commit_message>
<xml_diff>
--- a/docs/Controle de Ações - A3_ MMTES.xlsx
+++ b/docs/Controle de Ações - A3_ MMTES.xlsx
@@ -11,18 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="49">
   <si>
-    <t>PROJETO</t>
+    <t>GRUPO</t>
   </si>
   <si>
-    <t>INTEGRANTE</t>
+    <t>NOME</t>
   </si>
   <si>
-    <t>ATIVIDADE</t>
+    <t>RITO</t>
   </si>
   <si>
-    <t>REALIZAÇÃO</t>
+    <t>TAREFA</t>
   </si>
   <si>
     <t>DATA</t>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Finalização da segunda versão do App</t>
+  </si>
+  <si>
+    <t>Daniel Jones Marques, Marco Túlio Salvador</t>
+  </si>
+  <si>
+    <t>Finalização da Apresentação Canvas</t>
   </si>
   <si>
     <t>Observação 1: Todos os traços "-" na coluna B, referente ao nome do responsável pela ação/tarefa realizada, significam que todos os membros contribuiram para a execução.</t>
@@ -1557,11 +1563,21 @@
       <c r="Y28" s="10"/>
     </row>
     <row r="29">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="12"/>
+      <c r="A29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="17">
+        <v>45431.0</v>
+      </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -1611,14 +1627,10 @@
       <c r="Y30" s="10"/>
     </row>
     <row r="31">
-      <c r="A31" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="12"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -1642,6 +1654,12 @@
       <c r="Y31" s="10"/>
     </row>
     <row r="32">
+      <c r="A32" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="12"/>
@@ -1742,8 +1760,6 @@
       <c r="Y35" s="10"/>
     </row>
     <row r="36">
-      <c r="A36" s="6"/>
-      <c r="B36" s="15"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="12"/>
@@ -1795,11 +1811,11 @@
       <c r="X37" s="10"/>
       <c r="Y37" s="10"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
+    <row r="38">
+      <c r="A38" s="6"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="12"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -1908,7 +1924,7 @@
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -28147,14 +28163,41 @@
       <c r="X1013" s="10"/>
       <c r="Y1013" s="10"/>
     </row>
+    <row r="1014" ht="15.75" customHeight="1">
+      <c r="A1014" s="10"/>
+      <c r="B1014" s="10"/>
+      <c r="C1014" s="10"/>
+      <c r="D1014" s="10"/>
+      <c r="E1014" s="10"/>
+      <c r="F1014" s="10"/>
+      <c r="G1014" s="10"/>
+      <c r="H1014" s="10"/>
+      <c r="I1014" s="10"/>
+      <c r="J1014" s="10"/>
+      <c r="K1014" s="10"/>
+      <c r="L1014" s="10"/>
+      <c r="M1014" s="10"/>
+      <c r="N1014" s="10"/>
+      <c r="O1014" s="10"/>
+      <c r="P1014" s="10"/>
+      <c r="Q1014" s="10"/>
+      <c r="R1014" s="10"/>
+      <c r="S1014" s="10"/>
+      <c r="T1014" s="10"/>
+      <c r="U1014" s="10"/>
+      <c r="V1014" s="10"/>
+      <c r="W1014" s="10"/>
+      <c r="X1014" s="10"/>
+      <c r="Y1014" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="F2:F4"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
   </mergeCells>
-  <printOptions/>
+  <printOptions gridLines="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape"/>
   <drawing r:id="rId1"/>

</xml_diff>